<commit_message>
test: update test sheet
</commit_message>
<xml_diff>
--- a/test/data/test-modbus-uart-sheet.xlsx
+++ b/test/data/test-modbus-uart-sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
   <si>
     <t>tag</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>a2</t>
+  </si>
+  <si>
+    <t>INT</t>
   </si>
   <si>
     <t>a3</t>
@@ -278,18 +281,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -631,7 +628,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -655,16 +652,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -673,99 +670,93 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -1299,7 +1290,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1334,445 +1325,445 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>100</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>3</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>100</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>2</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
         <v>3</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>100</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>4</v>
       </c>
-      <c r="F5" s="3">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2">
         <v>3</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>5</v>
       </c>
-      <c r="F6" s="3">
-        <v>4</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>2</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2">
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>100</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>6</v>
       </c>
-      <c r="F7" s="3">
-        <v>5</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
         <v>2</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2">
         <v>3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>100</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>7</v>
       </c>
-      <c r="F8" s="3">
-        <v>6</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
         <v>2</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2">
         <v>3</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>100</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>8</v>
       </c>
-      <c r="F9" s="3">
-        <v>7</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
         <v>2</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2">
         <v>3</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>100</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>9</v>
       </c>
-      <c r="F10" s="3">
-        <v>8</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
         <v>2</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2">
         <v>3</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>100</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>10</v>
       </c>
-      <c r="F11" s="3">
-        <v>9</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
         <v>2</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2">
         <v>3</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>100</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>11</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="3">
-        <v>2</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2">
         <v>3</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>100</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>12</v>
       </c>
-      <c r="F13" s="3">
-        <v>11</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
         <v>2</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2">
         <v>3</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>100</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>13</v>
       </c>
-      <c r="F14" s="3">
-        <v>12</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
         <v>2</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2">
         <v>3</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>100</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>14</v>
       </c>
-      <c r="F15" s="3">
-        <v>13</v>
-      </c>
-      <c r="G15" s="3">
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
         <v>2</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2">
         <v>3</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>100</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>15</v>
       </c>
-      <c r="F16" s="3">
-        <v>14</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
         <v>2</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dev: fix concurrent map; remove site config
</commit_message>
<xml_diff>
--- a/test/data/test-modbus-uart-sheet.xlsx
+++ b/test/data/test-modbus-uart-sheet.xlsx
@@ -755,7 +755,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -763,6 +763,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1293,7 +1296,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J1" sqref="J$1:J$1048576"/>
+      <selection activeCell="A1" sqref="A1:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1366,7 +1369,7 @@
       <c r="I2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1398,7 +1401,7 @@
       <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1430,7 +1433,7 @@
       <c r="I4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1462,7 +1465,7 @@
       <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1494,7 +1497,7 @@
       <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1526,7 +1529,7 @@
       <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1558,7 +1561,7 @@
       <c r="I8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1590,7 +1593,7 @@
       <c r="I9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1622,7 +1625,7 @@
       <c r="I10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1654,7 +1657,7 @@
       <c r="I11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1686,7 +1689,7 @@
       <c r="I12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1718,7 +1721,7 @@
       <c r="I13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1750,7 +1753,7 @@
       <c r="I14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1782,7 +1785,7 @@
       <c r="I15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1814,7 +1817,7 @@
       <c r="I16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>